<commit_message>
Adding a lot of new experiment results
</commit_message>
<xml_diff>
--- a/results/epsilon/nim/Nim_EpsilonResults_100kGames_WithPolicySize.xlsx
+++ b/results/epsilon/nim/Nim_EpsilonResults_100kGames_WithPolicySize.xlsx
@@ -8,13 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="Nim_EpsilonResults_100kGames_Wi" sheetId="1" r:id="rId1"/>
+    <sheet name="Graph" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Epsilon</t>
   </si>
@@ -25,10 +26,13 @@
     <t>NimLoss</t>
   </si>
   <si>
-    <t>NimDraw</t>
+    <t>StatesInPolicy</t>
   </si>
   <si>
-    <t>StatesInPolicy</t>
+    <t>Win Rate</t>
+  </si>
+  <si>
+    <t>Loss Rate</t>
   </si>
 </sst>
 </file>
@@ -469,7 +473,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -512,11 +516,13 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="42" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -556,6 +562,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Percent" xfId="42" builtinId="5"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
@@ -568,6 +575,1417 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Nim_EpsilonResults_100kGames_Wi!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Win Rate</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Nim_EpsilonResults_100kGames_Wi!$A$2:$A$102</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="101"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9.9999999999999895E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.109999999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.119999999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.12999999999999901</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.13999999999999899</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.17</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.18</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.19</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.21</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.22</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.23</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.24</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.26</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.27</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.28000000000000003</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.28999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.31</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.32</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.33</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.34</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.36</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.37</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.38</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.39</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.41</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.42</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.43</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.44</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.46</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.47</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.48</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.49</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.51</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.52</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.53</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.54</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.56000000000000005</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.56999999999999995</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.57999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.59</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.61</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.62</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.63</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.64</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.66</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.67</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.68</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.69</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.71</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.72</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.73</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.74</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.76</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.77</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0.78</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.79</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0.81</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0.82</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0.84</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0.86</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0.87</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0.88</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0.89</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>0.91</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0.92</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0.93</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0.94</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0.96</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0.97</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0.98</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Nim_EpsilonResults_100kGames_Wi!$D$2:$D$102</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="101"/>
+                <c:pt idx="0">
+                  <c:v>0.63593</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.75300999999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.78847999999999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.76368000000000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.78559999999999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.76495000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.76700999999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.75521000000000005</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.77178000000000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.75956000000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.76566999999999996</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.77027999999999996</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.75566999999999995</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.75960000000000005</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.75292999999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.74966999999999995</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.75582000000000005</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.74583999999999995</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.74104000000000003</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.74970000000000003</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.74870000000000003</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.72867999999999999</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.74114999999999998</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.70843</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.72543999999999997</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.73111000000000004</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.72108000000000005</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.72121999999999997</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.71862999999999999</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.71462999999999999</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.71358999999999995</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.71711000000000003</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.71318000000000004</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.70474999999999999</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.70970999999999995</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.69559000000000004</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.70116000000000001</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.69887999999999995</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.69804999999999995</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.68728</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.68647000000000002</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.67927999999999999</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.67996999999999996</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.68422000000000005</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.67839000000000005</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.67749999999999999</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.67610000000000003</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.66925999999999997</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.66581000000000001</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.66883000000000004</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.66656000000000004</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.66147999999999996</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.64970000000000006</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.65125999999999995</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.65024000000000004</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.64478999999999997</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.65020999999999995</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.64014000000000004</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.64341999999999999</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.63778999999999997</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.63400999999999996</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.63114999999999999</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.63268999999999997</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.62710999999999995</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.61656</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.61646000000000001</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.61465999999999998</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.61477999999999999</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.60962000000000005</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.60696000000000006</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.60538999999999998</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.60038999999999998</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.59670999999999996</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.59699000000000002</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.58987999999999996</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.59053</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.58572999999999997</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.58125000000000004</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0.57552000000000003</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.57508000000000004</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.57237000000000005</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0.56813000000000002</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0.56618999999999997</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0.56054000000000004</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0.55683000000000005</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0.55689</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0.55398999999999998</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0.54559999999999997</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0.54612000000000005</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0.53859999999999997</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0.53683000000000003</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>0.53364999999999996</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0.52986999999999995</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0.52571000000000001</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0.52217000000000002</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0.52087000000000006</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0.51473999999999998</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0.51143000000000005</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0.50946999999999998</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>0.50158999999999998</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>0.50097000000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Nim_EpsilonResults_100kGames_Wi!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Loss Rate</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Nim_EpsilonResults_100kGames_Wi!$A$2:$A$102</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="101"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9.9999999999999895E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.109999999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.119999999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.12999999999999901</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.13999999999999899</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.17</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.18</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.19</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.21</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.22</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.23</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.24</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.26</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.27</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.28000000000000003</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.28999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.31</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.32</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.33</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.34</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.36</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.37</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.38</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.39</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.41</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.42</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.43</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.44</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.46</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.47</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.48</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.49</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.51</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.52</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.53</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.54</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.56000000000000005</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.56999999999999995</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.57999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.59</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.61</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.62</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.63</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.64</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.66</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.67</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.68</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.69</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.71</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.72</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.73</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.74</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.76</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.77</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0.78</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.79</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0.81</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0.82</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0.84</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0.86</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0.87</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0.88</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0.89</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>0.91</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0.92</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0.93</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0.94</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0.96</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0.97</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0.98</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Nim_EpsilonResults_100kGames_Wi!$E$2:$E$102</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="101"/>
+                <c:pt idx="0">
+                  <c:v>0.36407</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.24698999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.21152000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.23632</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.21440000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.23505000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.23299</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.24479000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.22822000000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.24043999999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.23433000000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.22972000000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.24432999999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.2404</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.24707000000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.25033</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.24418000000000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.25416</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.25896000000000002</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.25030000000000002</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.25130000000000002</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.27132000000000001</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.25885000000000002</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.29157</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.27456000000000003</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.26889000000000002</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.27892</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.27877999999999997</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.28137000000000001</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.28537000000000001</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.28641</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.28288999999999997</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.28682000000000002</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.29525000000000001</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.29028999999999999</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.30441000000000001</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.29883999999999999</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.30112</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.30195</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.31272</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.31352999999999998</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.32072000000000001</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.32002999999999998</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.31578000000000001</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.32161000000000001</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.32250000000000001</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.32390000000000002</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.33073999999999998</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.33418999999999999</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.33117000000000002</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.33344000000000001</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.33851999999999999</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.3503</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.34873999999999999</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.34976000000000002</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.35521000000000003</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.34978999999999999</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.35986000000000001</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.35658000000000001</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.36220999999999998</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.36598999999999998</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.36885000000000001</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.36731000000000003</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.37289</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.38344</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.38353999999999999</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.38534000000000002</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.38522000000000001</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.39038</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.39304</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.39461000000000002</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.39961000000000002</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.40328999999999998</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.40300999999999998</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.41011999999999998</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.40947</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.41427000000000003</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.41875000000000001</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0.42448000000000002</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.42492000000000002</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.42763000000000001</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0.43186999999999998</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0.43380999999999997</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0.43946000000000002</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0.44317000000000001</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0.44311</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0.44601000000000002</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0.45440000000000003</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0.45388000000000001</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0.46139999999999998</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0.46317000000000003</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>0.46634999999999999</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0.47012999999999999</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0.47428999999999999</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0.47782999999999998</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0.47913</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0.48526000000000002</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0.48857</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0.49053000000000002</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>0.49841000000000002</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>0.49902999999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="159889664"/>
+        <c:axId val="193297024"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="159889664"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="193297024"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:tickLblSkip val="5"/>
+        <c:tickMarkSkip val="5"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="193297024"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="159889664"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>15875</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>3175</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -857,13 +2275,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E102"/>
+  <dimension ref="A1:F102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="4" width="8.7265625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.7265625" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -873,14 +2295,17 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0</v>
       </c>
@@ -890,14 +2315,19 @@
       <c r="C2">
         <v>36407</v>
       </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
+      <c r="D2" s="1">
+        <f>B2/100000</f>
+        <v>0.63593</v>
+      </c>
+      <c r="E2" s="1">
+        <f>C2/100000</f>
+        <v>0.36407</v>
+      </c>
+      <c r="F2">
         <v>479</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>0.01</v>
       </c>
@@ -907,14 +2337,19 @@
       <c r="C3">
         <v>24699</v>
       </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
+      <c r="D3" s="1">
+        <f t="shared" ref="D3:D66" si="0">B3/100000</f>
+        <v>0.75300999999999996</v>
+      </c>
+      <c r="E3" s="1">
+        <f t="shared" ref="E3:E66" si="1">C3/100000</f>
+        <v>0.24698999999999999</v>
+      </c>
+      <c r="F3">
         <v>508</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>0.02</v>
       </c>
@@ -924,14 +2359,19 @@
       <c r="C4">
         <v>21152</v>
       </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D4" s="1">
+        <f t="shared" si="0"/>
+        <v>0.78847999999999996</v>
+      </c>
+      <c r="E4" s="1">
+        <f t="shared" si="1"/>
+        <v>0.21152000000000001</v>
+      </c>
+      <c r="F4">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>0.03</v>
       </c>
@@ -941,14 +2381,19 @@
       <c r="C5">
         <v>23632</v>
       </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D5" s="1">
+        <f t="shared" si="0"/>
+        <v>0.76368000000000003</v>
+      </c>
+      <c r="E5" s="1">
+        <f t="shared" si="1"/>
+        <v>0.23632</v>
+      </c>
+      <c r="F5">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>0.04</v>
       </c>
@@ -958,14 +2403,19 @@
       <c r="C6">
         <v>21440</v>
       </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D6" s="1">
+        <f t="shared" si="0"/>
+        <v>0.78559999999999997</v>
+      </c>
+      <c r="E6" s="1">
+        <f t="shared" si="1"/>
+        <v>0.21440000000000001</v>
+      </c>
+      <c r="F6">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>0.05</v>
       </c>
@@ -975,14 +2425,19 @@
       <c r="C7">
         <v>23505</v>
       </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D7" s="1">
+        <f t="shared" si="0"/>
+        <v>0.76495000000000002</v>
+      </c>
+      <c r="E7" s="1">
+        <f t="shared" si="1"/>
+        <v>0.23505000000000001</v>
+      </c>
+      <c r="F7">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>0.06</v>
       </c>
@@ -992,14 +2447,19 @@
       <c r="C8">
         <v>23299</v>
       </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.76700999999999997</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" si="1"/>
+        <v>0.23299</v>
+      </c>
+      <c r="F8">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>7.0000000000000007E-2</v>
       </c>
@@ -1009,14 +2469,19 @@
       <c r="C9">
         <v>24479</v>
       </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D9" s="1">
+        <f t="shared" si="0"/>
+        <v>0.75521000000000005</v>
+      </c>
+      <c r="E9" s="1">
+        <f t="shared" si="1"/>
+        <v>0.24479000000000001</v>
+      </c>
+      <c r="F9">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>0.08</v>
       </c>
@@ -1026,14 +2491,19 @@
       <c r="C10">
         <v>22822</v>
       </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D10" s="1">
+        <f t="shared" si="0"/>
+        <v>0.77178000000000002</v>
+      </c>
+      <c r="E10" s="1">
+        <f t="shared" si="1"/>
+        <v>0.22822000000000001</v>
+      </c>
+      <c r="F10">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>0.09</v>
       </c>
@@ -1043,14 +2513,19 @@
       <c r="C11">
         <v>24044</v>
       </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D11" s="1">
+        <f t="shared" si="0"/>
+        <v>0.75956000000000001</v>
+      </c>
+      <c r="E11" s="1">
+        <f t="shared" si="1"/>
+        <v>0.24043999999999999</v>
+      </c>
+      <c r="F11">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>9.9999999999999895E-2</v>
       </c>
@@ -1060,14 +2535,19 @@
       <c r="C12">
         <v>23433</v>
       </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
+      <c r="D12" s="1">
+        <f t="shared" si="0"/>
+        <v>0.76566999999999996</v>
+      </c>
+      <c r="E12" s="1">
+        <f t="shared" si="1"/>
+        <v>0.23433000000000001</v>
+      </c>
+      <c r="F12">
         <v>510</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>0.109999999999999</v>
       </c>
@@ -1077,14 +2557,19 @@
       <c r="C13">
         <v>22972</v>
       </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D13" s="1">
+        <f t="shared" si="0"/>
+        <v>0.77027999999999996</v>
+      </c>
+      <c r="E13" s="1">
+        <f t="shared" si="1"/>
+        <v>0.22972000000000001</v>
+      </c>
+      <c r="F13">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>0.119999999999999</v>
       </c>
@@ -1094,14 +2579,19 @@
       <c r="C14">
         <v>24433</v>
       </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D14" s="1">
+        <f t="shared" si="0"/>
+        <v>0.75566999999999995</v>
+      </c>
+      <c r="E14" s="1">
+        <f t="shared" si="1"/>
+        <v>0.24432999999999999</v>
+      </c>
+      <c r="F14">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>0.12999999999999901</v>
       </c>
@@ -1111,14 +2601,19 @@
       <c r="C15">
         <v>24040</v>
       </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D15" s="1">
+        <f t="shared" si="0"/>
+        <v>0.75960000000000005</v>
+      </c>
+      <c r="E15" s="1">
+        <f t="shared" si="1"/>
+        <v>0.2404</v>
+      </c>
+      <c r="F15">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>0.13999999999999899</v>
       </c>
@@ -1128,14 +2623,19 @@
       <c r="C16">
         <v>24707</v>
       </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D16" s="1">
+        <f t="shared" si="0"/>
+        <v>0.75292999999999999</v>
+      </c>
+      <c r="E16" s="1">
+        <f t="shared" si="1"/>
+        <v>0.24707000000000001</v>
+      </c>
+      <c r="F16">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>0.15</v>
       </c>
@@ -1145,14 +2645,19 @@
       <c r="C17">
         <v>25033</v>
       </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D17" s="1">
+        <f t="shared" si="0"/>
+        <v>0.74966999999999995</v>
+      </c>
+      <c r="E17" s="1">
+        <f t="shared" si="1"/>
+        <v>0.25033</v>
+      </c>
+      <c r="F17">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>0.16</v>
       </c>
@@ -1162,14 +2667,19 @@
       <c r="C18">
         <v>24418</v>
       </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D18" s="1">
+        <f t="shared" si="0"/>
+        <v>0.75582000000000005</v>
+      </c>
+      <c r="E18" s="1">
+        <f t="shared" si="1"/>
+        <v>0.24418000000000001</v>
+      </c>
+      <c r="F18">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>0.17</v>
       </c>
@@ -1179,14 +2689,19 @@
       <c r="C19">
         <v>25416</v>
       </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D19" s="1">
+        <f t="shared" si="0"/>
+        <v>0.74583999999999995</v>
+      </c>
+      <c r="E19" s="1">
+        <f t="shared" si="1"/>
+        <v>0.25416</v>
+      </c>
+      <c r="F19">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>0.18</v>
       </c>
@@ -1196,14 +2711,19 @@
       <c r="C20">
         <v>25896</v>
       </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D20" s="1">
+        <f t="shared" si="0"/>
+        <v>0.74104000000000003</v>
+      </c>
+      <c r="E20" s="1">
+        <f t="shared" si="1"/>
+        <v>0.25896000000000002</v>
+      </c>
+      <c r="F20">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>0.19</v>
       </c>
@@ -1213,14 +2733,19 @@
       <c r="C21">
         <v>25030</v>
       </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D21" s="1">
+        <f t="shared" si="0"/>
+        <v>0.74970000000000003</v>
+      </c>
+      <c r="E21" s="1">
+        <f t="shared" si="1"/>
+        <v>0.25030000000000002</v>
+      </c>
+      <c r="F21">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>0.2</v>
       </c>
@@ -1230,14 +2755,19 @@
       <c r="C22">
         <v>25130</v>
       </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="E22">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D22" s="1">
+        <f t="shared" si="0"/>
+        <v>0.74870000000000003</v>
+      </c>
+      <c r="E22" s="1">
+        <f t="shared" si="1"/>
+        <v>0.25130000000000002</v>
+      </c>
+      <c r="F22">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>0.21</v>
       </c>
@@ -1247,14 +2777,19 @@
       <c r="C23">
         <v>27132</v>
       </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="E23">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D23" s="1">
+        <f t="shared" si="0"/>
+        <v>0.72867999999999999</v>
+      </c>
+      <c r="E23" s="1">
+        <f t="shared" si="1"/>
+        <v>0.27132000000000001</v>
+      </c>
+      <c r="F23">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>0.22</v>
       </c>
@@ -1264,14 +2799,19 @@
       <c r="C24">
         <v>25885</v>
       </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-      <c r="E24">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D24" s="1">
+        <f t="shared" si="0"/>
+        <v>0.74114999999999998</v>
+      </c>
+      <c r="E24" s="1">
+        <f t="shared" si="1"/>
+        <v>0.25885000000000002</v>
+      </c>
+      <c r="F24">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>0.23</v>
       </c>
@@ -1281,14 +2821,19 @@
       <c r="C25">
         <v>29157</v>
       </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
-      <c r="E25">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D25" s="1">
+        <f t="shared" si="0"/>
+        <v>0.70843</v>
+      </c>
+      <c r="E25" s="1">
+        <f t="shared" si="1"/>
+        <v>0.29157</v>
+      </c>
+      <c r="F25">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>0.24</v>
       </c>
@@ -1298,14 +2843,19 @@
       <c r="C26">
         <v>27456</v>
       </c>
-      <c r="D26">
-        <v>0</v>
-      </c>
-      <c r="E26">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D26" s="1">
+        <f t="shared" si="0"/>
+        <v>0.72543999999999997</v>
+      </c>
+      <c r="E26" s="1">
+        <f t="shared" si="1"/>
+        <v>0.27456000000000003</v>
+      </c>
+      <c r="F26">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>0.25</v>
       </c>
@@ -1315,14 +2865,19 @@
       <c r="C27">
         <v>26889</v>
       </c>
-      <c r="D27">
-        <v>0</v>
-      </c>
-      <c r="E27">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D27" s="1">
+        <f t="shared" si="0"/>
+        <v>0.73111000000000004</v>
+      </c>
+      <c r="E27" s="1">
+        <f t="shared" si="1"/>
+        <v>0.26889000000000002</v>
+      </c>
+      <c r="F27">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>0.26</v>
       </c>
@@ -1332,14 +2887,19 @@
       <c r="C28">
         <v>27892</v>
       </c>
-      <c r="D28">
-        <v>0</v>
-      </c>
-      <c r="E28">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D28" s="1">
+        <f t="shared" si="0"/>
+        <v>0.72108000000000005</v>
+      </c>
+      <c r="E28" s="1">
+        <f t="shared" si="1"/>
+        <v>0.27892</v>
+      </c>
+      <c r="F28">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>0.27</v>
       </c>
@@ -1349,14 +2909,19 @@
       <c r="C29">
         <v>27878</v>
       </c>
-      <c r="D29">
-        <v>0</v>
-      </c>
-      <c r="E29">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D29" s="1">
+        <f t="shared" si="0"/>
+        <v>0.72121999999999997</v>
+      </c>
+      <c r="E29" s="1">
+        <f t="shared" si="1"/>
+        <v>0.27877999999999997</v>
+      </c>
+      <c r="F29">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>0.28000000000000003</v>
       </c>
@@ -1366,14 +2931,19 @@
       <c r="C30">
         <v>28137</v>
       </c>
-      <c r="D30">
-        <v>0</v>
-      </c>
-      <c r="E30">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D30" s="1">
+        <f t="shared" si="0"/>
+        <v>0.71862999999999999</v>
+      </c>
+      <c r="E30" s="1">
+        <f t="shared" si="1"/>
+        <v>0.28137000000000001</v>
+      </c>
+      <c r="F30">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>0.28999999999999998</v>
       </c>
@@ -1383,14 +2953,19 @@
       <c r="C31">
         <v>28537</v>
       </c>
-      <c r="D31">
-        <v>0</v>
-      </c>
-      <c r="E31">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D31" s="1">
+        <f t="shared" si="0"/>
+        <v>0.71462999999999999</v>
+      </c>
+      <c r="E31" s="1">
+        <f t="shared" si="1"/>
+        <v>0.28537000000000001</v>
+      </c>
+      <c r="F31">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>0.3</v>
       </c>
@@ -1400,14 +2975,19 @@
       <c r="C32">
         <v>28641</v>
       </c>
-      <c r="D32">
-        <v>0</v>
-      </c>
-      <c r="E32">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D32" s="1">
+        <f t="shared" si="0"/>
+        <v>0.71358999999999995</v>
+      </c>
+      <c r="E32" s="1">
+        <f t="shared" si="1"/>
+        <v>0.28641</v>
+      </c>
+      <c r="F32">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>0.31</v>
       </c>
@@ -1417,14 +2997,19 @@
       <c r="C33">
         <v>28289</v>
       </c>
-      <c r="D33">
-        <v>0</v>
-      </c>
-      <c r="E33">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D33" s="1">
+        <f t="shared" si="0"/>
+        <v>0.71711000000000003</v>
+      </c>
+      <c r="E33" s="1">
+        <f t="shared" si="1"/>
+        <v>0.28288999999999997</v>
+      </c>
+      <c r="F33">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>0.32</v>
       </c>
@@ -1434,14 +3019,19 @@
       <c r="C34">
         <v>28682</v>
       </c>
-      <c r="D34">
-        <v>0</v>
-      </c>
-      <c r="E34">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D34" s="1">
+        <f t="shared" si="0"/>
+        <v>0.71318000000000004</v>
+      </c>
+      <c r="E34" s="1">
+        <f t="shared" si="1"/>
+        <v>0.28682000000000002</v>
+      </c>
+      <c r="F34">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>0.33</v>
       </c>
@@ -1451,14 +3041,19 @@
       <c r="C35">
         <v>29525</v>
       </c>
-      <c r="D35">
-        <v>0</v>
-      </c>
-      <c r="E35">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D35" s="1">
+        <f t="shared" si="0"/>
+        <v>0.70474999999999999</v>
+      </c>
+      <c r="E35" s="1">
+        <f t="shared" si="1"/>
+        <v>0.29525000000000001</v>
+      </c>
+      <c r="F35">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>0.34</v>
       </c>
@@ -1468,14 +3063,19 @@
       <c r="C36">
         <v>29029</v>
       </c>
-      <c r="D36">
-        <v>0</v>
-      </c>
-      <c r="E36">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D36" s="1">
+        <f t="shared" si="0"/>
+        <v>0.70970999999999995</v>
+      </c>
+      <c r="E36" s="1">
+        <f t="shared" si="1"/>
+        <v>0.29028999999999999</v>
+      </c>
+      <c r="F36">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>0.35</v>
       </c>
@@ -1485,14 +3085,19 @@
       <c r="C37">
         <v>30441</v>
       </c>
-      <c r="D37">
-        <v>0</v>
-      </c>
-      <c r="E37">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D37" s="1">
+        <f t="shared" si="0"/>
+        <v>0.69559000000000004</v>
+      </c>
+      <c r="E37" s="1">
+        <f t="shared" si="1"/>
+        <v>0.30441000000000001</v>
+      </c>
+      <c r="F37">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>0.36</v>
       </c>
@@ -1502,14 +3107,19 @@
       <c r="C38">
         <v>29884</v>
       </c>
-      <c r="D38">
-        <v>0</v>
-      </c>
-      <c r="E38">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D38" s="1">
+        <f t="shared" si="0"/>
+        <v>0.70116000000000001</v>
+      </c>
+      <c r="E38" s="1">
+        <f t="shared" si="1"/>
+        <v>0.29883999999999999</v>
+      </c>
+      <c r="F38">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>0.37</v>
       </c>
@@ -1519,14 +3129,19 @@
       <c r="C39">
         <v>30112</v>
       </c>
-      <c r="D39">
-        <v>0</v>
-      </c>
-      <c r="E39">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D39" s="1">
+        <f t="shared" si="0"/>
+        <v>0.69887999999999995</v>
+      </c>
+      <c r="E39" s="1">
+        <f t="shared" si="1"/>
+        <v>0.30112</v>
+      </c>
+      <c r="F39">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>0.38</v>
       </c>
@@ -1536,14 +3151,19 @@
       <c r="C40">
         <v>30195</v>
       </c>
-      <c r="D40">
-        <v>0</v>
-      </c>
-      <c r="E40">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D40" s="1">
+        <f t="shared" si="0"/>
+        <v>0.69804999999999995</v>
+      </c>
+      <c r="E40" s="1">
+        <f t="shared" si="1"/>
+        <v>0.30195</v>
+      </c>
+      <c r="F40">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>0.39</v>
       </c>
@@ -1553,14 +3173,19 @@
       <c r="C41">
         <v>31272</v>
       </c>
-      <c r="D41">
-        <v>0</v>
-      </c>
-      <c r="E41">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D41" s="1">
+        <f t="shared" si="0"/>
+        <v>0.68728</v>
+      </c>
+      <c r="E41" s="1">
+        <f t="shared" si="1"/>
+        <v>0.31272</v>
+      </c>
+      <c r="F41">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>0.4</v>
       </c>
@@ -1570,14 +3195,19 @@
       <c r="C42">
         <v>31353</v>
       </c>
-      <c r="D42">
-        <v>0</v>
-      </c>
-      <c r="E42">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D42" s="1">
+        <f t="shared" si="0"/>
+        <v>0.68647000000000002</v>
+      </c>
+      <c r="E42" s="1">
+        <f t="shared" si="1"/>
+        <v>0.31352999999999998</v>
+      </c>
+      <c r="F42">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>0.41</v>
       </c>
@@ -1587,14 +3217,19 @@
       <c r="C43">
         <v>32072</v>
       </c>
-      <c r="D43">
-        <v>0</v>
-      </c>
-      <c r="E43">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D43" s="1">
+        <f t="shared" si="0"/>
+        <v>0.67927999999999999</v>
+      </c>
+      <c r="E43" s="1">
+        <f t="shared" si="1"/>
+        <v>0.32072000000000001</v>
+      </c>
+      <c r="F43">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>0.42</v>
       </c>
@@ -1604,14 +3239,19 @@
       <c r="C44">
         <v>32003</v>
       </c>
-      <c r="D44">
-        <v>0</v>
-      </c>
-      <c r="E44">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D44" s="1">
+        <f t="shared" si="0"/>
+        <v>0.67996999999999996</v>
+      </c>
+      <c r="E44" s="1">
+        <f t="shared" si="1"/>
+        <v>0.32002999999999998</v>
+      </c>
+      <c r="F44">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>0.43</v>
       </c>
@@ -1621,14 +3261,19 @@
       <c r="C45">
         <v>31578</v>
       </c>
-      <c r="D45">
-        <v>0</v>
-      </c>
-      <c r="E45">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D45" s="1">
+        <f t="shared" si="0"/>
+        <v>0.68422000000000005</v>
+      </c>
+      <c r="E45" s="1">
+        <f t="shared" si="1"/>
+        <v>0.31578000000000001</v>
+      </c>
+      <c r="F45">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>0.44</v>
       </c>
@@ -1638,14 +3283,19 @@
       <c r="C46">
         <v>32161</v>
       </c>
-      <c r="D46">
-        <v>0</v>
-      </c>
-      <c r="E46">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D46" s="1">
+        <f t="shared" si="0"/>
+        <v>0.67839000000000005</v>
+      </c>
+      <c r="E46" s="1">
+        <f t="shared" si="1"/>
+        <v>0.32161000000000001</v>
+      </c>
+      <c r="F46">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>0.45</v>
       </c>
@@ -1655,14 +3305,19 @@
       <c r="C47">
         <v>32250</v>
       </c>
-      <c r="D47">
-        <v>0</v>
-      </c>
-      <c r="E47">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D47" s="1">
+        <f t="shared" si="0"/>
+        <v>0.67749999999999999</v>
+      </c>
+      <c r="E47" s="1">
+        <f t="shared" si="1"/>
+        <v>0.32250000000000001</v>
+      </c>
+      <c r="F47">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>0.46</v>
       </c>
@@ -1672,14 +3327,19 @@
       <c r="C48">
         <v>32390</v>
       </c>
-      <c r="D48">
-        <v>0</v>
-      </c>
-      <c r="E48">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D48" s="1">
+        <f t="shared" si="0"/>
+        <v>0.67610000000000003</v>
+      </c>
+      <c r="E48" s="1">
+        <f t="shared" si="1"/>
+        <v>0.32390000000000002</v>
+      </c>
+      <c r="F48">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>0.47</v>
       </c>
@@ -1689,14 +3349,19 @@
       <c r="C49">
         <v>33074</v>
       </c>
-      <c r="D49">
-        <v>0</v>
-      </c>
-      <c r="E49">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D49" s="1">
+        <f t="shared" si="0"/>
+        <v>0.66925999999999997</v>
+      </c>
+      <c r="E49" s="1">
+        <f t="shared" si="1"/>
+        <v>0.33073999999999998</v>
+      </c>
+      <c r="F49">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>0.48</v>
       </c>
@@ -1706,14 +3371,19 @@
       <c r="C50">
         <v>33419</v>
       </c>
-      <c r="D50">
-        <v>0</v>
-      </c>
-      <c r="E50">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D50" s="1">
+        <f t="shared" si="0"/>
+        <v>0.66581000000000001</v>
+      </c>
+      <c r="E50" s="1">
+        <f t="shared" si="1"/>
+        <v>0.33418999999999999</v>
+      </c>
+      <c r="F50">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>0.49</v>
       </c>
@@ -1723,14 +3393,19 @@
       <c r="C51">
         <v>33117</v>
       </c>
-      <c r="D51">
-        <v>0</v>
-      </c>
-      <c r="E51">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D51" s="1">
+        <f t="shared" si="0"/>
+        <v>0.66883000000000004</v>
+      </c>
+      <c r="E51" s="1">
+        <f t="shared" si="1"/>
+        <v>0.33117000000000002</v>
+      </c>
+      <c r="F51">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>0.5</v>
       </c>
@@ -1740,14 +3415,19 @@
       <c r="C52">
         <v>33344</v>
       </c>
-      <c r="D52">
-        <v>0</v>
-      </c>
-      <c r="E52">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D52" s="1">
+        <f t="shared" si="0"/>
+        <v>0.66656000000000004</v>
+      </c>
+      <c r="E52" s="1">
+        <f t="shared" si="1"/>
+        <v>0.33344000000000001</v>
+      </c>
+      <c r="F52">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>0.51</v>
       </c>
@@ -1757,14 +3437,19 @@
       <c r="C53">
         <v>33852</v>
       </c>
-      <c r="D53">
-        <v>0</v>
-      </c>
-      <c r="E53">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D53" s="1">
+        <f t="shared" si="0"/>
+        <v>0.66147999999999996</v>
+      </c>
+      <c r="E53" s="1">
+        <f t="shared" si="1"/>
+        <v>0.33851999999999999</v>
+      </c>
+      <c r="F53">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>0.52</v>
       </c>
@@ -1774,14 +3459,19 @@
       <c r="C54">
         <v>35030</v>
       </c>
-      <c r="D54">
-        <v>0</v>
-      </c>
-      <c r="E54">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D54" s="1">
+        <f t="shared" si="0"/>
+        <v>0.64970000000000006</v>
+      </c>
+      <c r="E54" s="1">
+        <f t="shared" si="1"/>
+        <v>0.3503</v>
+      </c>
+      <c r="F54">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>0.53</v>
       </c>
@@ -1791,14 +3481,19 @@
       <c r="C55">
         <v>34874</v>
       </c>
-      <c r="D55">
-        <v>0</v>
-      </c>
-      <c r="E55">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D55" s="1">
+        <f t="shared" si="0"/>
+        <v>0.65125999999999995</v>
+      </c>
+      <c r="E55" s="1">
+        <f t="shared" si="1"/>
+        <v>0.34873999999999999</v>
+      </c>
+      <c r="F55">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>0.54</v>
       </c>
@@ -1808,14 +3503,19 @@
       <c r="C56">
         <v>34976</v>
       </c>
-      <c r="D56">
-        <v>0</v>
-      </c>
-      <c r="E56">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D56" s="1">
+        <f t="shared" si="0"/>
+        <v>0.65024000000000004</v>
+      </c>
+      <c r="E56" s="1">
+        <f t="shared" si="1"/>
+        <v>0.34976000000000002</v>
+      </c>
+      <c r="F56">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>0.55000000000000004</v>
       </c>
@@ -1825,14 +3525,19 @@
       <c r="C57">
         <v>35521</v>
       </c>
-      <c r="D57">
-        <v>0</v>
-      </c>
-      <c r="E57">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D57" s="1">
+        <f t="shared" si="0"/>
+        <v>0.64478999999999997</v>
+      </c>
+      <c r="E57" s="1">
+        <f t="shared" si="1"/>
+        <v>0.35521000000000003</v>
+      </c>
+      <c r="F57">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>0.56000000000000005</v>
       </c>
@@ -1842,14 +3547,19 @@
       <c r="C58">
         <v>34979</v>
       </c>
-      <c r="D58">
-        <v>0</v>
-      </c>
-      <c r="E58">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D58" s="1">
+        <f t="shared" si="0"/>
+        <v>0.65020999999999995</v>
+      </c>
+      <c r="E58" s="1">
+        <f t="shared" si="1"/>
+        <v>0.34978999999999999</v>
+      </c>
+      <c r="F58">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>0.56999999999999995</v>
       </c>
@@ -1859,14 +3569,19 @@
       <c r="C59">
         <v>35986</v>
       </c>
-      <c r="D59">
-        <v>0</v>
-      </c>
-      <c r="E59">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D59" s="1">
+        <f t="shared" si="0"/>
+        <v>0.64014000000000004</v>
+      </c>
+      <c r="E59" s="1">
+        <f t="shared" si="1"/>
+        <v>0.35986000000000001</v>
+      </c>
+      <c r="F59">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>0.57999999999999996</v>
       </c>
@@ -1876,14 +3591,19 @@
       <c r="C60">
         <v>35658</v>
       </c>
-      <c r="D60">
-        <v>0</v>
-      </c>
-      <c r="E60">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D60" s="1">
+        <f t="shared" si="0"/>
+        <v>0.64341999999999999</v>
+      </c>
+      <c r="E60" s="1">
+        <f t="shared" si="1"/>
+        <v>0.35658000000000001</v>
+      </c>
+      <c r="F60">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>0.59</v>
       </c>
@@ -1893,14 +3613,19 @@
       <c r="C61">
         <v>36221</v>
       </c>
-      <c r="D61">
-        <v>0</v>
-      </c>
-      <c r="E61">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D61" s="1">
+        <f t="shared" si="0"/>
+        <v>0.63778999999999997</v>
+      </c>
+      <c r="E61" s="1">
+        <f t="shared" si="1"/>
+        <v>0.36220999999999998</v>
+      </c>
+      <c r="F61">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>0.6</v>
       </c>
@@ -1910,14 +3635,19 @@
       <c r="C62">
         <v>36599</v>
       </c>
-      <c r="D62">
-        <v>0</v>
-      </c>
-      <c r="E62">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D62" s="1">
+        <f t="shared" si="0"/>
+        <v>0.63400999999999996</v>
+      </c>
+      <c r="E62" s="1">
+        <f t="shared" si="1"/>
+        <v>0.36598999999999998</v>
+      </c>
+      <c r="F62">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>0.61</v>
       </c>
@@ -1927,14 +3657,19 @@
       <c r="C63">
         <v>36885</v>
       </c>
-      <c r="D63">
-        <v>0</v>
-      </c>
-      <c r="E63">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D63" s="1">
+        <f t="shared" si="0"/>
+        <v>0.63114999999999999</v>
+      </c>
+      <c r="E63" s="1">
+        <f t="shared" si="1"/>
+        <v>0.36885000000000001</v>
+      </c>
+      <c r="F63">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>0.62</v>
       </c>
@@ -1944,14 +3679,19 @@
       <c r="C64">
         <v>36731</v>
       </c>
-      <c r="D64">
-        <v>0</v>
-      </c>
-      <c r="E64">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D64" s="1">
+        <f t="shared" si="0"/>
+        <v>0.63268999999999997</v>
+      </c>
+      <c r="E64" s="1">
+        <f t="shared" si="1"/>
+        <v>0.36731000000000003</v>
+      </c>
+      <c r="F64">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>0.63</v>
       </c>
@@ -1961,14 +3701,19 @@
       <c r="C65">
         <v>37289</v>
       </c>
-      <c r="D65">
-        <v>0</v>
-      </c>
-      <c r="E65">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D65" s="1">
+        <f t="shared" si="0"/>
+        <v>0.62710999999999995</v>
+      </c>
+      <c r="E65" s="1">
+        <f t="shared" si="1"/>
+        <v>0.37289</v>
+      </c>
+      <c r="F65">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>0.64</v>
       </c>
@@ -1978,14 +3723,19 @@
       <c r="C66">
         <v>38344</v>
       </c>
-      <c r="D66">
-        <v>0</v>
-      </c>
-      <c r="E66">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D66" s="1">
+        <f t="shared" si="0"/>
+        <v>0.61656</v>
+      </c>
+      <c r="E66" s="1">
+        <f t="shared" si="1"/>
+        <v>0.38344</v>
+      </c>
+      <c r="F66">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>0.65</v>
       </c>
@@ -1995,14 +3745,19 @@
       <c r="C67">
         <v>38354</v>
       </c>
-      <c r="D67">
-        <v>0</v>
-      </c>
-      <c r="E67">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D67" s="1">
+        <f t="shared" ref="D67:D102" si="2">B67/100000</f>
+        <v>0.61646000000000001</v>
+      </c>
+      <c r="E67" s="1">
+        <f t="shared" ref="E67:E102" si="3">C67/100000</f>
+        <v>0.38353999999999999</v>
+      </c>
+      <c r="F67">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>0.66</v>
       </c>
@@ -2012,14 +3767,19 @@
       <c r="C68">
         <v>38534</v>
       </c>
-      <c r="D68">
-        <v>0</v>
-      </c>
-      <c r="E68">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D68" s="1">
+        <f t="shared" si="2"/>
+        <v>0.61465999999999998</v>
+      </c>
+      <c r="E68" s="1">
+        <f t="shared" si="3"/>
+        <v>0.38534000000000002</v>
+      </c>
+      <c r="F68">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>0.67</v>
       </c>
@@ -2029,14 +3789,19 @@
       <c r="C69">
         <v>38522</v>
       </c>
-      <c r="D69">
-        <v>0</v>
-      </c>
-      <c r="E69">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D69" s="1">
+        <f t="shared" si="2"/>
+        <v>0.61477999999999999</v>
+      </c>
+      <c r="E69" s="1">
+        <f t="shared" si="3"/>
+        <v>0.38522000000000001</v>
+      </c>
+      <c r="F69">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>0.68</v>
       </c>
@@ -2046,14 +3811,19 @@
       <c r="C70">
         <v>39038</v>
       </c>
-      <c r="D70">
-        <v>0</v>
-      </c>
-      <c r="E70">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D70" s="1">
+        <f t="shared" si="2"/>
+        <v>0.60962000000000005</v>
+      </c>
+      <c r="E70" s="1">
+        <f t="shared" si="3"/>
+        <v>0.39038</v>
+      </c>
+      <c r="F70">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>0.69</v>
       </c>
@@ -2063,14 +3833,19 @@
       <c r="C71">
         <v>39304</v>
       </c>
-      <c r="D71">
-        <v>0</v>
-      </c>
-      <c r="E71">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D71" s="1">
+        <f t="shared" si="2"/>
+        <v>0.60696000000000006</v>
+      </c>
+      <c r="E71" s="1">
+        <f t="shared" si="3"/>
+        <v>0.39304</v>
+      </c>
+      <c r="F71">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>0.7</v>
       </c>
@@ -2080,14 +3855,19 @@
       <c r="C72">
         <v>39461</v>
       </c>
-      <c r="D72">
-        <v>0</v>
-      </c>
-      <c r="E72">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D72" s="1">
+        <f t="shared" si="2"/>
+        <v>0.60538999999999998</v>
+      </c>
+      <c r="E72" s="1">
+        <f t="shared" si="3"/>
+        <v>0.39461000000000002</v>
+      </c>
+      <c r="F72">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>0.71</v>
       </c>
@@ -2097,14 +3877,19 @@
       <c r="C73">
         <v>39961</v>
       </c>
-      <c r="D73">
-        <v>0</v>
-      </c>
-      <c r="E73">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D73" s="1">
+        <f t="shared" si="2"/>
+        <v>0.60038999999999998</v>
+      </c>
+      <c r="E73" s="1">
+        <f t="shared" si="3"/>
+        <v>0.39961000000000002</v>
+      </c>
+      <c r="F73">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>0.72</v>
       </c>
@@ -2114,14 +3899,19 @@
       <c r="C74">
         <v>40329</v>
       </c>
-      <c r="D74">
-        <v>0</v>
-      </c>
-      <c r="E74">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D74" s="1">
+        <f t="shared" si="2"/>
+        <v>0.59670999999999996</v>
+      </c>
+      <c r="E74" s="1">
+        <f t="shared" si="3"/>
+        <v>0.40328999999999998</v>
+      </c>
+      <c r="F74">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>0.73</v>
       </c>
@@ -2131,14 +3921,19 @@
       <c r="C75">
         <v>40301</v>
       </c>
-      <c r="D75">
-        <v>0</v>
-      </c>
-      <c r="E75">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D75" s="1">
+        <f t="shared" si="2"/>
+        <v>0.59699000000000002</v>
+      </c>
+      <c r="E75" s="1">
+        <f t="shared" si="3"/>
+        <v>0.40300999999999998</v>
+      </c>
+      <c r="F75">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>0.74</v>
       </c>
@@ -2148,14 +3943,19 @@
       <c r="C76">
         <v>41012</v>
       </c>
-      <c r="D76">
-        <v>0</v>
-      </c>
-      <c r="E76">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D76" s="1">
+        <f t="shared" si="2"/>
+        <v>0.58987999999999996</v>
+      </c>
+      <c r="E76" s="1">
+        <f t="shared" si="3"/>
+        <v>0.41011999999999998</v>
+      </c>
+      <c r="F76">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>0.75</v>
       </c>
@@ -2165,14 +3965,19 @@
       <c r="C77">
         <v>40947</v>
       </c>
-      <c r="D77">
-        <v>0</v>
-      </c>
-      <c r="E77">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D77" s="1">
+        <f t="shared" si="2"/>
+        <v>0.59053</v>
+      </c>
+      <c r="E77" s="1">
+        <f t="shared" si="3"/>
+        <v>0.40947</v>
+      </c>
+      <c r="F77">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>0.76</v>
       </c>
@@ -2182,14 +3987,19 @@
       <c r="C78">
         <v>41427</v>
       </c>
-      <c r="D78">
-        <v>0</v>
-      </c>
-      <c r="E78">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D78" s="1">
+        <f t="shared" si="2"/>
+        <v>0.58572999999999997</v>
+      </c>
+      <c r="E78" s="1">
+        <f t="shared" si="3"/>
+        <v>0.41427000000000003</v>
+      </c>
+      <c r="F78">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>0.77</v>
       </c>
@@ -2199,14 +4009,19 @@
       <c r="C79">
         <v>41875</v>
       </c>
-      <c r="D79">
-        <v>0</v>
-      </c>
-      <c r="E79">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D79" s="1">
+        <f t="shared" si="2"/>
+        <v>0.58125000000000004</v>
+      </c>
+      <c r="E79" s="1">
+        <f t="shared" si="3"/>
+        <v>0.41875000000000001</v>
+      </c>
+      <c r="F79">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>0.78</v>
       </c>
@@ -2216,14 +4031,19 @@
       <c r="C80">
         <v>42448</v>
       </c>
-      <c r="D80">
-        <v>0</v>
-      </c>
-      <c r="E80">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D80" s="1">
+        <f t="shared" si="2"/>
+        <v>0.57552000000000003</v>
+      </c>
+      <c r="E80" s="1">
+        <f t="shared" si="3"/>
+        <v>0.42448000000000002</v>
+      </c>
+      <c r="F80">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>0.79</v>
       </c>
@@ -2233,14 +4053,19 @@
       <c r="C81">
         <v>42492</v>
       </c>
-      <c r="D81">
-        <v>0</v>
-      </c>
-      <c r="E81">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D81" s="1">
+        <f t="shared" si="2"/>
+        <v>0.57508000000000004</v>
+      </c>
+      <c r="E81" s="1">
+        <f t="shared" si="3"/>
+        <v>0.42492000000000002</v>
+      </c>
+      <c r="F81">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>0.8</v>
       </c>
@@ -2250,14 +4075,19 @@
       <c r="C82">
         <v>42763</v>
       </c>
-      <c r="D82">
-        <v>0</v>
-      </c>
-      <c r="E82">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D82" s="1">
+        <f t="shared" si="2"/>
+        <v>0.57237000000000005</v>
+      </c>
+      <c r="E82" s="1">
+        <f t="shared" si="3"/>
+        <v>0.42763000000000001</v>
+      </c>
+      <c r="F82">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>0.81</v>
       </c>
@@ -2267,14 +4097,19 @@
       <c r="C83">
         <v>43187</v>
       </c>
-      <c r="D83">
-        <v>0</v>
-      </c>
-      <c r="E83">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D83" s="1">
+        <f t="shared" si="2"/>
+        <v>0.56813000000000002</v>
+      </c>
+      <c r="E83" s="1">
+        <f t="shared" si="3"/>
+        <v>0.43186999999999998</v>
+      </c>
+      <c r="F83">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>0.82</v>
       </c>
@@ -2284,14 +4119,19 @@
       <c r="C84">
         <v>43381</v>
       </c>
-      <c r="D84">
-        <v>0</v>
-      </c>
-      <c r="E84">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D84" s="1">
+        <f t="shared" si="2"/>
+        <v>0.56618999999999997</v>
+      </c>
+      <c r="E84" s="1">
+        <f t="shared" si="3"/>
+        <v>0.43380999999999997</v>
+      </c>
+      <c r="F84">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>0.83</v>
       </c>
@@ -2301,14 +4141,19 @@
       <c r="C85">
         <v>43946</v>
       </c>
-      <c r="D85">
-        <v>0</v>
-      </c>
-      <c r="E85">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D85" s="1">
+        <f t="shared" si="2"/>
+        <v>0.56054000000000004</v>
+      </c>
+      <c r="E85" s="1">
+        <f t="shared" si="3"/>
+        <v>0.43946000000000002</v>
+      </c>
+      <c r="F85">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>0.84</v>
       </c>
@@ -2318,14 +4163,19 @@
       <c r="C86">
         <v>44317</v>
       </c>
-      <c r="D86">
-        <v>0</v>
-      </c>
-      <c r="E86">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D86" s="1">
+        <f t="shared" si="2"/>
+        <v>0.55683000000000005</v>
+      </c>
+      <c r="E86" s="1">
+        <f t="shared" si="3"/>
+        <v>0.44317000000000001</v>
+      </c>
+      <c r="F86">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>0.85</v>
       </c>
@@ -2335,14 +4185,19 @@
       <c r="C87">
         <v>44311</v>
       </c>
-      <c r="D87">
-        <v>0</v>
-      </c>
-      <c r="E87">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D87" s="1">
+        <f t="shared" si="2"/>
+        <v>0.55689</v>
+      </c>
+      <c r="E87" s="1">
+        <f t="shared" si="3"/>
+        <v>0.44311</v>
+      </c>
+      <c r="F87">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>0.86</v>
       </c>
@@ -2352,14 +4207,19 @@
       <c r="C88">
         <v>44601</v>
       </c>
-      <c r="D88">
-        <v>0</v>
-      </c>
-      <c r="E88">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D88" s="1">
+        <f t="shared" si="2"/>
+        <v>0.55398999999999998</v>
+      </c>
+      <c r="E88" s="1">
+        <f t="shared" si="3"/>
+        <v>0.44601000000000002</v>
+      </c>
+      <c r="F88">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>0.87</v>
       </c>
@@ -2369,14 +4229,19 @@
       <c r="C89">
         <v>45440</v>
       </c>
-      <c r="D89">
-        <v>0</v>
-      </c>
-      <c r="E89">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D89" s="1">
+        <f t="shared" si="2"/>
+        <v>0.54559999999999997</v>
+      </c>
+      <c r="E89" s="1">
+        <f t="shared" si="3"/>
+        <v>0.45440000000000003</v>
+      </c>
+      <c r="F89">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>0.88</v>
       </c>
@@ -2386,14 +4251,19 @@
       <c r="C90">
         <v>45388</v>
       </c>
-      <c r="D90">
-        <v>0</v>
-      </c>
-      <c r="E90">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D90" s="1">
+        <f t="shared" si="2"/>
+        <v>0.54612000000000005</v>
+      </c>
+      <c r="E90" s="1">
+        <f t="shared" si="3"/>
+        <v>0.45388000000000001</v>
+      </c>
+      <c r="F90">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>0.89</v>
       </c>
@@ -2403,14 +4273,19 @@
       <c r="C91">
         <v>46140</v>
       </c>
-      <c r="D91">
-        <v>0</v>
-      </c>
-      <c r="E91">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D91" s="1">
+        <f t="shared" si="2"/>
+        <v>0.53859999999999997</v>
+      </c>
+      <c r="E91" s="1">
+        <f t="shared" si="3"/>
+        <v>0.46139999999999998</v>
+      </c>
+      <c r="F91">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>0.9</v>
       </c>
@@ -2420,14 +4295,19 @@
       <c r="C92">
         <v>46317</v>
       </c>
-      <c r="D92">
-        <v>0</v>
-      </c>
-      <c r="E92">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D92" s="1">
+        <f t="shared" si="2"/>
+        <v>0.53683000000000003</v>
+      </c>
+      <c r="E92" s="1">
+        <f t="shared" si="3"/>
+        <v>0.46317000000000003</v>
+      </c>
+      <c r="F92">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>0.91</v>
       </c>
@@ -2437,14 +4317,19 @@
       <c r="C93">
         <v>46635</v>
       </c>
-      <c r="D93">
-        <v>0</v>
-      </c>
-      <c r="E93">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D93" s="1">
+        <f t="shared" si="2"/>
+        <v>0.53364999999999996</v>
+      </c>
+      <c r="E93" s="1">
+        <f t="shared" si="3"/>
+        <v>0.46634999999999999</v>
+      </c>
+      <c r="F93">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>0.92</v>
       </c>
@@ -2454,14 +4339,19 @@
       <c r="C94">
         <v>47013</v>
       </c>
-      <c r="D94">
-        <v>0</v>
-      </c>
-      <c r="E94">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D94" s="1">
+        <f t="shared" si="2"/>
+        <v>0.52986999999999995</v>
+      </c>
+      <c r="E94" s="1">
+        <f t="shared" si="3"/>
+        <v>0.47012999999999999</v>
+      </c>
+      <c r="F94">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>0.93</v>
       </c>
@@ -2471,14 +4361,19 @@
       <c r="C95">
         <v>47429</v>
       </c>
-      <c r="D95">
-        <v>0</v>
-      </c>
-      <c r="E95">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D95" s="1">
+        <f t="shared" si="2"/>
+        <v>0.52571000000000001</v>
+      </c>
+      <c r="E95" s="1">
+        <f t="shared" si="3"/>
+        <v>0.47428999999999999</v>
+      </c>
+      <c r="F95">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>0.94</v>
       </c>
@@ -2488,14 +4383,19 @@
       <c r="C96">
         <v>47783</v>
       </c>
-      <c r="D96">
-        <v>0</v>
-      </c>
-      <c r="E96">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D96" s="1">
+        <f t="shared" si="2"/>
+        <v>0.52217000000000002</v>
+      </c>
+      <c r="E96" s="1">
+        <f t="shared" si="3"/>
+        <v>0.47782999999999998</v>
+      </c>
+      <c r="F96">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>0.95</v>
       </c>
@@ -2505,14 +4405,19 @@
       <c r="C97">
         <v>47913</v>
       </c>
-      <c r="D97">
-        <v>0</v>
-      </c>
-      <c r="E97">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D97" s="1">
+        <f t="shared" si="2"/>
+        <v>0.52087000000000006</v>
+      </c>
+      <c r="E97" s="1">
+        <f t="shared" si="3"/>
+        <v>0.47913</v>
+      </c>
+      <c r="F97">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A98">
         <v>0.96</v>
       </c>
@@ -2522,14 +4427,19 @@
       <c r="C98">
         <v>48526</v>
       </c>
-      <c r="D98">
-        <v>0</v>
-      </c>
-      <c r="E98">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D98" s="1">
+        <f t="shared" si="2"/>
+        <v>0.51473999999999998</v>
+      </c>
+      <c r="E98" s="1">
+        <f t="shared" si="3"/>
+        <v>0.48526000000000002</v>
+      </c>
+      <c r="F98">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A99">
         <v>0.97</v>
       </c>
@@ -2539,14 +4449,19 @@
       <c r="C99">
         <v>48857</v>
       </c>
-      <c r="D99">
-        <v>0</v>
-      </c>
-      <c r="E99">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D99" s="1">
+        <f t="shared" si="2"/>
+        <v>0.51143000000000005</v>
+      </c>
+      <c r="E99" s="1">
+        <f t="shared" si="3"/>
+        <v>0.48857</v>
+      </c>
+      <c r="F99">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A100">
         <v>0.98</v>
       </c>
@@ -2556,14 +4471,19 @@
       <c r="C100">
         <v>49053</v>
       </c>
-      <c r="D100">
-        <v>0</v>
-      </c>
-      <c r="E100">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D100" s="1">
+        <f t="shared" si="2"/>
+        <v>0.50946999999999998</v>
+      </c>
+      <c r="E100" s="1">
+        <f t="shared" si="3"/>
+        <v>0.49053000000000002</v>
+      </c>
+      <c r="F100">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A101">
         <v>0.99</v>
       </c>
@@ -2573,14 +4493,19 @@
       <c r="C101">
         <v>49841</v>
       </c>
-      <c r="D101">
-        <v>0</v>
-      </c>
-      <c r="E101">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D101" s="1">
+        <f t="shared" si="2"/>
+        <v>0.50158999999999998</v>
+      </c>
+      <c r="E101" s="1">
+        <f t="shared" si="3"/>
+        <v>0.49841000000000002</v>
+      </c>
+      <c r="F101">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A102">
         <v>1</v>
       </c>
@@ -2590,14 +4515,34 @@
       <c r="C102">
         <v>49903</v>
       </c>
-      <c r="D102">
-        <v>0</v>
-      </c>
-      <c r="E102">
+      <c r="D102" s="1">
+        <f t="shared" si="2"/>
+        <v>0.50097000000000003</v>
+      </c>
+      <c r="E102" s="1">
+        <f t="shared" si="3"/>
+        <v>0.49902999999999997</v>
+      </c>
+      <c r="F102">
         <v>511</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>